<commit_message>
planilha de product backlog atualizada da sprint3
</commit_message>
<xml_diff>
--- a/Documentos/PRODUCT BACKLOG - ESTIMATIVA.xlsx
+++ b/Documentos/PRODUCT BACKLOG - ESTIMATIVA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b442170cbd8b6ddd/Área de Trabalho/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e1327c28a9523567/Documentos/ColdTech/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="170" documentId="8_{C1378E02-2A2B-40EA-B317-09DBF6DAF538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4046E7EC-229A-40EE-BEEE-98A527D11B55}"/>
+  <xr:revisionPtr revIDLastSave="206" documentId="8_{C1378E02-2A2B-40EA-B317-09DBF6DAF538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F23B4EDD-B7D5-47A7-8E94-D4FF9FD20618}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="116">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -307,6 +307,84 @@
   </si>
   <si>
     <t>Atualizar Script de Criação do Banco</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>Manual de instalação</t>
+  </si>
+  <si>
+    <t>Manual de instalação dos sensores</t>
+  </si>
+  <si>
+    <t>SP3C</t>
+  </si>
+  <si>
+    <t>5-P</t>
+  </si>
+  <si>
+    <t>Cadastro conectado no BD</t>
+  </si>
+  <si>
+    <t>Login conectado no BD</t>
+  </si>
+  <si>
+    <t>Dashboard conectado no BD</t>
+  </si>
+  <si>
+    <t>13-G</t>
+  </si>
+  <si>
+    <t>Integração do cadastro com API e banco de dados</t>
+  </si>
+  <si>
+    <t>Integração do login com API e banco de dados</t>
+  </si>
+  <si>
+    <t>Integração da dashboard com API e banco de dados</t>
+  </si>
+  <si>
+    <t>Fluxograma</t>
+  </si>
+  <si>
+    <t>8-M</t>
+  </si>
+  <si>
+    <t>Fluxo de atendimento ao cliente</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>Teste integrado do analytics</t>
+  </si>
+  <si>
+    <t>Alertas na dashboard</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>Teste integrado da solução de IoT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integragração do arduino com o branco e usuário via WLAN </t>
+  </si>
+  <si>
+    <t>21-GG</t>
   </si>
 </sst>
 </file>
@@ -686,10 +764,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -966,8 +1040,8 @@
   <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1657,56 +1731,203 @@
     </row>
     <row r="31" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
+      <c r="B31" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="G31" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="H31" s="34" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="32" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
-    </row>
-    <row r="33" spans="1:1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="G32" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="H32" s="34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
-    </row>
-    <row r="34" spans="1:1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="G33" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="H33" s="34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
-    </row>
-    <row r="35" spans="1:1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="G34" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="H34" s="34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
-    </row>
-    <row r="36" spans="1:1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="G35" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="H35" s="34" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
-    </row>
-    <row r="37" spans="1:1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="G36" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="H36" s="34" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
-    </row>
-    <row r="38" spans="1:1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="G37" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="H37" s="34" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
     </row>
-    <row r="39" spans="1:1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
     </row>
-    <row r="40" spans="1:1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
     </row>
-    <row r="41" spans="1:1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6"/>
     </row>
-    <row r="42" spans="1:1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6"/>
     </row>
-    <row r="43" spans="1:1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
     </row>
-    <row r="44" spans="1:1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6"/>
     </row>
-    <row r="45" spans="1:1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6"/>
     </row>
-    <row r="46" spans="1:1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6"/>
     </row>
-    <row r="47" spans="1:1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
     </row>
-    <row r="48" spans="1:1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6"/>
     </row>
     <row r="49" spans="1:1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
@@ -1744,23 +1965,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3e7a52f9-5c66-44a9-86f3-38766607b952" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100678EE90E01C1554D81095FA0DFA567B7" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aa8a4c4165da3897a30e8f01da5d8f69">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3e7a52f9-5c66-44a9-86f3-38766607b952" xmlns:ns4="bba0be46-aa14-4462-94e7-e7f5e4df92a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="91c5418c5803fd5ab2167d9c9a7cb239" ns3:_="" ns4:_="">
     <xsd:import namespace="3e7a52f9-5c66-44a9-86f3-38766607b952"/>
@@ -1949,10 +2153,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3e7a52f9-5c66-44a9-86f3-38766607b952" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4D1CD5-6433-4ACC-8229-288768F65B94}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E84921C-6EC4-4CA6-8AF2-7C2C0DF4C39F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3e7a52f9-5c66-44a9-86f3-38766607b952"/>
+    <ds:schemaRef ds:uri="bba0be46-aa14-4462-94e7-e7f5e4df92a1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1975,20 +2207,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E84921C-6EC4-4CA6-8AF2-7C2C0DF4C39F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4D1CD5-6433-4ACC-8229-288768F65B94}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3e7a52f9-5c66-44a9-86f3-38766607b952"/>
-    <ds:schemaRef ds:uri="bba0be46-aa14-4462-94e7-e7f5e4df92a1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>